<commit_message>
did 2 more user tests
</commit_message>
<xml_diff>
--- a/Individual Project Documents/User Test Results.xlsx
+++ b/Individual Project Documents/User Test Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\Work\Bristol Uni\Year 4\Individual-Project-and-Innovation-Case\Individual Project Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Year 4\Individual-Project-and-Innovation-Case\Individual Project Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42193A0-E60F-4488-A02A-3918053338C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DFA1CB-42F1-4367-AEC7-A3BB9D4393D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31500" yWindow="2460" windowWidth="21600" windowHeight="15435" xr2:uid="{5C0D2622-50FB-4B76-AAFB-BE2A30450EBD}"/>
+    <workbookView xWindow="21300" yWindow="5130" windowWidth="7500" windowHeight="6000" xr2:uid="{5C0D2622-50FB-4B76-AAFB-BE2A30450EBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
   <si>
     <t>User 1 - Tom</t>
   </si>
@@ -135,9 +135,6 @@
     <t>Beginner</t>
   </si>
   <si>
-    <t>Found hard to line up shot</t>
-  </si>
-  <si>
     <t>Yes it was very helpful, especially shot 5</t>
   </si>
   <si>
@@ -151,6 +148,51 @@
   </si>
   <si>
     <t>User 2 - Dan</t>
+  </si>
+  <si>
+    <t>Yes it was helpful as long I was able to line up the shot properly.</t>
+  </si>
+  <si>
+    <t>Having to move the objects, but most of all line up the shot using the cue marker.</t>
+  </si>
+  <si>
+    <t>That it explains it very well and that I hit more balls with it on</t>
+  </si>
+  <si>
+    <t>I think that it is very smart application and if it was easier to use it would be more welcomed but I wouldn’t use it myself as I found it too hard to move things into place and line up the shots.</t>
+  </si>
+  <si>
+    <t>I was wondering whether I was placing the bvall correctly or not as there is a lot of human error so I put a lot of focus on moving the ball maybe more than I should have just so it lines up correctly. The lines did help to visualise the shot a lot. When i usually play i do imaginary lines to line up my shots but with the hololens it displays them for me which i found useful.</t>
+  </si>
+  <si>
+    <t>It would be useful if it put everything in place for me!</t>
+  </si>
+  <si>
+    <t>Intermediate</t>
+  </si>
+  <si>
+    <t>Started to get a headache</t>
+  </si>
+  <si>
+    <t>Bounced off of extra cushion</t>
+  </si>
+  <si>
+    <t>Noted that cue ball did follow line</t>
+  </si>
+  <si>
+    <t>Yes for more difficult shots I had a better idea of where I had to aim. For the easier shots I didn’t really notice a difference.</t>
+  </si>
+  <si>
+    <t>Positioning the table is quite difficult as the table doesn’t fit on the screen all at the same time so you have to keep walking round adjusting each corner which messes up other bits.</t>
+  </si>
+  <si>
+    <t>Umm, the aim assist thing.</t>
+  </si>
+  <si>
+    <t>I think the headset is uncomfotable and a bit offputting  but the system it self is intuative and very helpful.</t>
+  </si>
+  <si>
+    <t>Because you cant see everything at once ou jhave to keep looking away from the ball to see where the target is. When you compare it to VR everything you see is hologram but having half hologram half normal world is a bit weird.</t>
   </si>
 </sst>
 </file>
@@ -189,7 +231,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,6 +250,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -221,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -231,6 +279,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -547,17 +599,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1038D93F-8FDE-4233-B74A-53B835EBF9C3}">
-  <dimension ref="A2:F45"/>
+  <dimension ref="A2:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="225" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
     <col min="5" max="7" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -566,7 +619,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>1</v>
@@ -600,7 +653,13 @@
       <c r="A6" t="s">
         <v>12</v>
       </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
       <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
         <v>32</v>
       </c>
       <c r="F6" s="5"/>
@@ -618,51 +677,62 @@
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="1"/>
       <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
+      <c r="B10" s="1"/>
       <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
+      <c r="B11" s="4"/>
       <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="B12" s="4"/>
       <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="B13" s="1"/>
       <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B14"/>
+      <c r="B14" s="4"/>
       <c r="C14"/>
       <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B15"/>
+      <c r="B15" s="4"/>
       <c r="C15"/>
       <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
@@ -670,10 +740,10 @@
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
     </row>
-    <row r="18" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>20</v>
       </c>
@@ -681,199 +751,320 @@
       <c r="C18"/>
       <c r="D18"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="5"/>
+      <c r="B19" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="D20" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="D21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="5"/>
+      <c r="B22" s="4"/>
       <c r="C22" s="5"/>
       <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="5"/>
+      <c r="B23" s="1"/>
       <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B24"/>
+      <c r="B24" s="4"/>
       <c r="C24"/>
       <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="B25" s="9"/>
       <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>6</v>
       </c>
+      <c r="B29" s="8">
+        <v>2</v>
+      </c>
       <c r="D29" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E29" s="8">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>7</v>
       </c>
-      <c r="B30"/>
+      <c r="B30" s="8">
+        <v>8</v>
+      </c>
       <c r="C30"/>
       <c r="D30" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>8</v>
       </c>
+      <c r="B31" s="8">
+        <v>0</v>
+      </c>
       <c r="D31" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>9</v>
       </c>
+      <c r="B32" s="8">
+        <v>15</v>
+      </c>
       <c r="D32" s="8">
         <v>15</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>10</v>
       </c>
+      <c r="B33" s="8">
+        <v>12</v>
+      </c>
       <c r="D33" s="8">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>11</v>
       </c>
+      <c r="B34" s="8">
+        <v>2</v>
+      </c>
       <c r="D34" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D35" s="8"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="8"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D36" s="8"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="8"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>23</v>
       </c>
+      <c r="B37" s="8">
+        <v>5</v>
+      </c>
       <c r="D37" s="8">
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
+      <c r="B38" s="8">
+        <v>6</v>
+      </c>
       <c r="D38" s="8">
         <v>8</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
+      <c r="B39" s="8">
+        <v>4</v>
+      </c>
       <c r="D39" s="8">
         <v>7</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
+      <c r="B40" s="8">
+        <v>7</v>
+      </c>
       <c r="D40" s="8">
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>27</v>
       </c>
+      <c r="B41" s="8">
+        <v>7</v>
+      </c>
       <c r="D41" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="E41" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>28</v>
       </c>
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
       <c r="D42" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="E42" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>29</v>
       </c>
+      <c r="B43" t="s">
+        <v>49</v>
+      </c>
       <c r="D43" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="E43" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>30</v>
       </c>
+      <c r="B44" t="s">
+        <v>50</v>
+      </c>
       <c r="D44" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="E44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>31</v>
       </c>
+      <c r="B45" t="s">
+        <v>51</v>
+      </c>
       <c r="D45" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="E45" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>52</v>
+      </c>
+      <c r="E46" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>